<commit_message>
Aggionata checklist ID 191, 376 non APPLICABILITA'
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#MDATECHNOLOGYSRLXX/MDA_TECHNOLOGY/SOILAB_Innovative/13.8.5/report-checklist.xlsx
+++ b/GATEWAY/A1#111#MDATECHNOLOGYSRLXX/MDA_TECHNOLOGY/SOILAB_Innovative/13.8.5/report-checklist.xlsx
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Summary!$A$1:$G$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$W$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$W$49</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="286">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -162,6 +162,15 @@
   </si>
   <si>
     <t>IDENTIFICATIVI SOFTWARE</t>
+  </si>
+  <si>
+    <t>subject_application_id:</t>
+  </si>
+  <si>
+    <t>subject_application_vendor:</t>
+  </si>
+  <si>
+    <t>subject_application_version:</t>
   </si>
   <si>
     <t>ID</t>
@@ -472,6 +481,12 @@
     <t>VALIDAZIONE_CDA2_RSA_CT23_KO</t>
   </si>
   <si>
+    <t>VALIDAZIONE_CDA2_LAB_TRASF_CT1</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LAB_TRASF_CT2</t>
+  </si>
+  <si>
     <t>ID TEST CASE OK</t>
   </si>
   <si>
@@ -618,6 +633,16 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
+    <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Laboratorio dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST- OK" riportata nei documenti "Caso di test - Trasfusionale" e "CDA2_Trasfusionale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Laboratorio dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST OK - HLA" riportata nei documenti "Caso di test - Trasfusionale" e "CDA2_Trasfusionale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
     <t>448, 449</t>
   </si>
   <si>
@@ -771,393 +796,340 @@
     <t>INVIO MANUALE DEL DOCUMENTO AL SERVIZIO DI VALIDAZIONE DEL GATEWAY A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO)</t>
   </si>
   <si>
+    <t>2025-10-16T10:42:07Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T08:53:41Z</t>
+  </si>
+  <si>
+    <t>2025-10-16T10:52:55Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T08:56:03Z</t>
+  </si>
+  <si>
+    <t>2025-10-16T10:53:05Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T08:58:10Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T09:00:02Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T09:02:11Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T09:11:29Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T09:16:41Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T09:31:45Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T09:41:53Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T10:28:04Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T12:22:17Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T12:26:48Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T12:30:02Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T12:33:33Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T12:37:13Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T12:41:38Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T12:46:02Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T12:51:54Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T14:58:17Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T15:22:09Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T15:28:18Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T15:43:18Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T15:59:44Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T16:05:29Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T16:09:38Z</t>
+  </si>
+  <si>
+    <t>2025-10-16T09:35:20Z</t>
+  </si>
+  <si>
+    <t>2025-10-16T09:37:11Z</t>
+  </si>
+  <si>
+    <t>2025-10-16T10:48:27Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T16:14:46Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T12:22:39Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T16:22:52Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T12:27:49Z</t>
+  </si>
+  <si>
+    <t>2025-10-15T16:27:21Z</t>
+  </si>
+  <si>
+    <t>23415566c0fd5a41051b2f3cb429b685</t>
+  </si>
+  <si>
+    <t>7cdd972f909199b7cf969f247f80ae34</t>
+  </si>
+  <si>
+    <t>d943f8de07709965b4467203b94a37d0</t>
+  </si>
+  <si>
+    <t>e05ce4874d0cfb8814b39ce0b36a0739</t>
+  </si>
+  <si>
+    <t>f546524c0e69d283aac939fb87f172ed</t>
+  </si>
+  <si>
+    <t>884c1d6e9ff9c26d7b96e6d8c20a9edb</t>
+  </si>
+  <si>
+    <t>35a4bc7155724acf980e85f25e7c7969</t>
+  </si>
+  <si>
+    <t>87a8d40f6b3223722bf70d2153f0124f</t>
+  </si>
+  <si>
+    <t>1baeb22a9c2c1fe8e0754cd22314cebf</t>
+  </si>
+  <si>
+    <t>7f7879141fccff4426aa98ec85084ca3</t>
+  </si>
+  <si>
+    <t>7853c0991f9b44f8bc7821f7e919fc39</t>
+  </si>
+  <si>
+    <t>ff61e964aca8dd7e7260d624aeef5a4d</t>
+  </si>
+  <si>
+    <t>0edfc93c1cd696b36ac7dc37cc3008db</t>
+  </si>
+  <si>
+    <t>91d7dc9c039d5dc9de34c63ada90a7f4</t>
+  </si>
+  <si>
+    <t>37ff83b0c282e8859d8f263488f7b50d</t>
+  </si>
+  <si>
+    <t>a59f2d258e9ebc574d9d3170b03d1d4e</t>
+  </si>
+  <si>
+    <t>5086e2375fa207217175139a6191a0d3</t>
+  </si>
+  <si>
+    <t>ef1b61615d3be2f32b6df8faa72b6951</t>
+  </si>
+  <si>
+    <t>ef417b2e0fa6037f644489928dd40cb1</t>
+  </si>
+  <si>
+    <t>0805af7d255f8afcea98aa52c96ce02d</t>
+  </si>
+  <si>
+    <t>ff15f57cdb17da1af93f2a9bae4d203d</t>
+  </si>
+  <si>
+    <t>9b3855011d8d6b08542e5ef1b3948b70</t>
+  </si>
+  <si>
+    <t>f10aceb5004aef0ee13ff5b8e160809b</t>
+  </si>
+  <si>
+    <t>173d149183b952f1a44886940802d846</t>
+  </si>
+  <si>
+    <t>65a2c55ce74b8bde3d402ff725346865</t>
+  </si>
+  <si>
+    <t>82432949d65a56f7f407ccc4a58c65df</t>
+  </si>
+  <si>
+    <t>e6d5ec29d396136306cb26a60e0f4163</t>
+  </si>
+  <si>
+    <t>219151b6e7ad35af6a949e6dae88298b</t>
+  </si>
+  <si>
+    <t>1f8c36a736d7f172510ae65eddd70a11</t>
+  </si>
+  <si>
+    <t>0ccdb11e0dee32b40bd14b8282327386</t>
+  </si>
+  <si>
+    <t>396cd6a75092fec34c6c9db2e6064d79</t>
+  </si>
+  <si>
+    <t>0cae1911fea5be0164e19dddae1532b4</t>
+  </si>
+  <si>
+    <t>26ac58ae79fef50ec8d94d34ab2cbd34</t>
+  </si>
+  <si>
+    <t>f046a0c84e6b3e7828a610bdcaf40816</t>
+  </si>
+  <si>
+    <t>673bc354ce00cf95ccdfb8b5cabd2184</t>
+  </si>
+  <si>
+    <t>ebe735caf9d8b82f6904e33aaac33fa8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.65f1f497be^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.3faa8cec92^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.ab0d58cd65^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.beac35acde^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.99ab8c5a15^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.57c2264f14^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.d4a057bc0b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.3760b29730^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.0565a5416c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.27b936a3c1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.5f1d107ac6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.e0ea002ad7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.9b0b5d5ada^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.3b6792579a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.1e0b5c231a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.e9a1e03a5d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.22431cff6e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.6167b4c870^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.3c4ff700e6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.5cbd158e59^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.c2cafc84cc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.daf7ac182f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.e98767e602^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.3f5665eab0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.0595430571^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.2445e27c04^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.8cde8f502c96af348d9a76d469863951151743345a904933eea192ddf8d8bc0c.72da0f36e6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.2a882cc8f3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.fe7e7c2e30^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.37957d3bdb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.01ede77c6d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.a1e76f7fad^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Fse2: Operazione non consentita a causa di dati nella richiesta incompleti o non validi</t>
+  </si>
+  <si>
+    <t>Fse2: Operazione non consentita a causa di dati della richiesta incompleti o non validi</t>
+  </si>
+  <si>
+    <t>Fse2: I servizi FSE non hanno risposto in tempo alla richiesta (TIMEOUT)</t>
+  </si>
+  <si>
+    <t>Fse2: Errore nei dati del file CDA</t>
+  </si>
+  <si>
     <t>Si procede alla sistemazione dei dati tramite intervento manuale e ritrasmissione del documento.</t>
   </si>
   <si>
     <t>Si eseguono altri tentativi di trasmissione del documento</t>
   </si>
   <si>
-    <t>Fse2: Operazione non consentita a causa di dati della richiesta incompleti o non validi</t>
-  </si>
-  <si>
-    <t>Fse2: Errore nei dati del file CDA</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Precondizioni:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Il fornitore utilizza un token jwt mancante di campi obbligatori, quindi non valido.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Descrizione di Business del caso di test: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" con un token jwt non valido a causa della mancanza di uno o più campi obbligatori al fine di testare la gestione dell'errore sul token (status code 403), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-Al fine di rendere non valido il token è necessario non valorizzare nel JWT il campo "purpose_of_use".</t>
-    </r>
-  </si>
-  <si>
-    <t>Fse2: I servizi FSE non hanno risposto in tempo alla richiesta (TIMEOUT)</t>
-  </si>
-  <si>
-    <t>subject_application_id: SOILAB Innovative</t>
-  </si>
-  <si>
-    <t>subject_application_vendor: MDA TECHNOLOGY</t>
-  </si>
-  <si>
-    <t>subject_application_version: 13.8.5</t>
-  </si>
-  <si>
-    <t>MDA TECHNOLOGY</t>
-  </si>
-  <si>
-    <t>2025-10-15T08:53:41Z</t>
-  </si>
-  <si>
-    <t>7cdd972f909199b7cf969f247f80ae34</t>
-  </si>
-  <si>
-    <t>2025-10-15T08:56:03Z</t>
-  </si>
-  <si>
-    <t>e05ce4874d0cfb8814b39ce0b36a0739</t>
-  </si>
-  <si>
-    <t>2025-10-15T08:58:10Z</t>
-  </si>
-  <si>
-    <t>884c1d6e9ff9c26d7b96e6d8c20a9edb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.3faa8cec92^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T09:00:02Z</t>
-  </si>
-  <si>
-    <t>35a4bc7155724acf980e85f25e7c7969</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.ab0d58cd65^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T09:02:11Z</t>
-  </si>
-  <si>
-    <t>87a8d40f6b3223722bf70d2153f0124f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.beac35acde^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T09:11:29Z</t>
-  </si>
-  <si>
-    <t>1baeb22a9c2c1fe8e0754cd22314cebf</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.99ab8c5a15^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T09:16:41Z</t>
-  </si>
-  <si>
-    <t>7f7879141fccff4426aa98ec85084ca3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.57c2264f14^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T09:31:45Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.d4a057bc0b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>7853c0991f9b44f8bc7821f7e919fc39</t>
-  </si>
-  <si>
-    <t>2025-10-15T09:41:53Z</t>
-  </si>
-  <si>
-    <t>ff61e964aca8dd7e7260d624aeef5a4d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.3760b29730^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T10:28:04Z</t>
-  </si>
-  <si>
-    <t>0edfc93c1cd696b36ac7dc37cc3008db</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.0565a5416c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>Fse2: Operazione non consentita a causa di dati nella richiesta incompleti o non validi</t>
-  </si>
-  <si>
-    <t>2025-10-15T12:22:39Z</t>
-  </si>
-  <si>
-    <t>26ac58ae79fef50ec8d94d34ab2cbd34</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.fe7e7c2e30^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T12:27:49Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.01ede77c6d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>673bc354ce00cf95ccdfb8b5cabd2184</t>
-  </si>
-  <si>
-    <t>2025-10-15T12:22:17Z</t>
-  </si>
-  <si>
-    <t>91d7dc9c039d5dc9de34c63ada90a7f4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.27b936a3c1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T12:26:48Z</t>
-  </si>
-  <si>
-    <t>37ff83b0c282e8859d8f263488f7b50d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.5f1d107ac6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T12:30:02Z</t>
-  </si>
-  <si>
-    <t>a59f2d258e9ebc574d9d3170b03d1d4e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.e0ea002ad7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T12:33:33Z</t>
-  </si>
-  <si>
-    <t>5086e2375fa207217175139a6191a0d3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.9b0b5d5ada^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T12:37:13Z</t>
-  </si>
-  <si>
-    <t>ef1b61615d3be2f32b6df8faa72b6951</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.3b6792579a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T12:41:38Z</t>
-  </si>
-  <si>
-    <t>ef417b2e0fa6037f644489928dd40cb1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.1e0b5c231a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T12:46:02Z</t>
-  </si>
-  <si>
-    <t>0805af7d255f8afcea98aa52c96ce02d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.e9a1e03a5d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T12:51:54Z</t>
-  </si>
-  <si>
-    <t>ff15f57cdb17da1af93f2a9bae4d203d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.22431cff6e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T14:58:17Z</t>
-  </si>
-  <si>
-    <t>9b3855011d8d6b08542e5ef1b3948b70</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.6167b4c870^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>f10aceb5004aef0ee13ff5b8e160809b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.3c4ff700e6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T15:22:09Z</t>
-  </si>
-  <si>
-    <t>2025-10-15T15:28:18Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.5cbd158e59^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>173d149183b952f1a44886940802d846</t>
-  </si>
-  <si>
-    <t>2025-10-15T15:43:18Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.c2cafc84cc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>65a2c55ce74b8bde3d402ff725346865</t>
-  </si>
-  <si>
-    <t>2025-10-15T15:59:44Z</t>
-  </si>
-  <si>
-    <t>82432949d65a56f7f407ccc4a58c65df</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.daf7ac182f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T16:05:29Z</t>
-  </si>
-  <si>
-    <t>e6d5ec29d396136306cb26a60e0f4163</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.e98767e602^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T16:09:38Z</t>
-  </si>
-  <si>
-    <t>219151b6e7ad35af6a949e6dae88298b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.3f5665eab0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T16:14:46Z</t>
-  </si>
-  <si>
-    <t>0cae1911fea5be0164e19dddae1532b4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.2a882cc8f3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T16:22:52Z</t>
-  </si>
-  <si>
-    <t>f046a0c84e6b3e7828a610bdcaf40816</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.37957d3bdb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-15T16:27:21Z</t>
-  </si>
-  <si>
-    <t>ebe735caf9d8b82f6904e33aaac33fa8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.a1e76f7fad^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>1f8c36a736d7f172510ae65eddd70a11</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.0595430571^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-16T09:35:20Z</t>
-  </si>
-  <si>
-    <t>0ccdb11e0dee32b40bd14b8282327386</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6b63deb6a4ea543dfa506fa67febc0f98fe087fea3d96287bb61d0d0f67c1c0b.2445e27c04^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-16T09:37:11Z</t>
-  </si>
-  <si>
-    <t>23415566c0fd5a41051b2f3cb429b685</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.c956da568a4959b2c3fd6d409612337256a481647c1b0fac278d78621533e9a6.65f1f497be^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-16T10:42:07Z</t>
-  </si>
-  <si>
-    <t>396cd6a75092fec34c6c9db2e6064d79</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.8cde8f502c96af348d9a76d469863951151743345a904933eea192ddf8d8bc0c.72da0f36e6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-10-16T10:48:27Z</t>
-  </si>
-  <si>
-    <t>d943f8de07709965b4467203b94a37d0</t>
-  </si>
-  <si>
-    <t>2025-10-16T10:52:55Z</t>
-  </si>
-  <si>
-    <t>2025-10-16T10:53:05Z</t>
-  </si>
-  <si>
-    <t>f546524c0e69d283aac939fb87f172ed</t>
+    <t>I laboratori di analisi che utilizzano il nostro software sono laboratori di base con settori specializzati di tipo ambulatoriale e non ospedaliero. Nei punti prelievo di questi laboratori accedono cittadini che devono fare controlli di prevenzione e in nessuno di essi sono svolte attività di trasfusione, per le quali servono specifici atti autorizzativi che non rientrano tra quelli in possesso dalla nostra clientela.</t>
   </si>
 </sst>
 </file>
@@ -1291,10 +1263,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1761,9 +1732,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2087,7 +2056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -2104,7 +2073,7 @@
     </row>
     <row r="2" spans="1:1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
@@ -2114,22 +2083,22 @@
     </row>
     <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="300" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -2227,7 +2196,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3233,13 +3202,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W607"/>
+  <dimension ref="A1:W609"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3285,9 +3254,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="49"/>
-      <c r="C2" s="50" t="s">
-        <v>177</v>
-      </c>
+      <c r="C2" s="50"/>
       <c r="D2" s="49"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -3314,7 +3281,7 @@
       </c>
       <c r="B3" s="52"/>
       <c r="C3" s="57" t="s">
-        <v>174</v>
+        <v>14</v>
       </c>
       <c r="D3" s="49"/>
       <c r="F3" s="6"/>
@@ -3340,7 +3307,7 @@
       <c r="A4" s="53"/>
       <c r="B4" s="54"/>
       <c r="C4" s="57" t="s">
-        <v>175</v>
+        <v>15</v>
       </c>
       <c r="D4" s="49"/>
       <c r="E4" s="4"/>
@@ -3367,7 +3334,7 @@
       <c r="A5" s="55"/>
       <c r="B5" s="56"/>
       <c r="C5" s="57" t="s">
-        <v>176</v>
+        <v>16</v>
       </c>
       <c r="D5" s="49"/>
       <c r="F5" s="6"/>
@@ -3457,73 +3424,73 @@
     </row>
     <row r="9" spans="1:23" s="18" customFormat="1" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L9" s="20" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="N9" s="20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="O9" s="20" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="P9" s="20" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Q9" s="20" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="R9" s="20" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="S9" s="20" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="T9" s="20" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="U9" s="21" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="V9" s="20" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="W9" s="22" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3531,31 +3498,31 @@
         <v>4</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="E10" s="43" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F10" s="36">
         <v>45946</v>
       </c>
       <c r="G10" s="36" t="s">
-        <v>275</v>
+        <v>174</v>
       </c>
       <c r="H10" s="36" t="s">
-        <v>273</v>
+        <v>210</v>
       </c>
       <c r="I10" s="37" t="s">
-        <v>274</v>
+        <v>246</v>
       </c>
       <c r="J10" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K10" s="38"/>
       <c r="L10" s="38"/>
@@ -3570,7 +3537,7 @@
       <c r="U10" s="39"/>
       <c r="V10" s="40"/>
       <c r="W10" s="38" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3578,60 +3545,60 @@
         <v>28</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C11" s="41" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E11" s="43" t="s">
-        <v>172</v>
-      </c>
-      <c r="F11" s="36">
+        <v>46</v>
+      </c>
+      <c r="F11" s="37">
         <v>45945</v>
       </c>
       <c r="G11" s="37" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H11" s="37" t="s">
-        <v>179</v>
+        <v>211</v>
       </c>
       <c r="I11" s="42" t="s">
-        <v>167</v>
+        <v>247</v>
       </c>
       <c r="J11" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K11" s="38"/>
       <c r="L11" s="38"/>
       <c r="M11" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N11" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O11" s="38" t="s">
-        <v>206</v>
+        <v>279</v>
       </c>
       <c r="P11" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q11" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R11" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S11" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T11" s="38"/>
       <c r="U11" s="39"/>
       <c r="V11" s="40"/>
       <c r="W11" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3639,60 +3606,60 @@
         <v>32</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C12" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="45">
+      <c r="F12" s="37">
         <v>45945</v>
       </c>
       <c r="G12" s="37" t="s">
-        <v>280</v>
+        <v>176</v>
       </c>
       <c r="H12" s="37" t="s">
-        <v>279</v>
+        <v>212</v>
       </c>
       <c r="I12" s="42" t="s">
-        <v>167</v>
+        <v>247</v>
       </c>
       <c r="J12" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K12" s="38"/>
       <c r="L12" s="38"/>
       <c r="M12" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N12" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O12" s="38" t="s">
-        <v>206</v>
+        <v>279</v>
       </c>
       <c r="P12" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q12" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R12" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S12" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T12" s="38"/>
       <c r="U12" s="39"/>
       <c r="V12" s="40"/>
       <c r="W12" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3700,60 +3667,60 @@
         <v>36</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E13" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="36">
+        <v>52</v>
+      </c>
+      <c r="F13" s="37">
         <v>45945</v>
       </c>
       <c r="G13" s="37" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H13" s="37" t="s">
-        <v>181</v>
+        <v>213</v>
       </c>
       <c r="I13" s="42" t="s">
-        <v>167</v>
+        <v>247</v>
       </c>
       <c r="J13" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K13" s="38"/>
       <c r="L13" s="38"/>
       <c r="M13" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N13" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O13" s="38" t="s">
-        <v>170</v>
+        <v>280</v>
       </c>
       <c r="P13" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q13" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R13" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S13" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T13" s="38"/>
       <c r="U13" s="39"/>
       <c r="V13" s="40"/>
       <c r="W13" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3761,60 +3728,60 @@
         <v>40</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E14" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="36">
+        <v>52</v>
+      </c>
+      <c r="F14" s="37">
         <v>45945</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>281</v>
+        <v>178</v>
       </c>
       <c r="H14" s="37" t="s">
-        <v>282</v>
+        <v>214</v>
       </c>
       <c r="I14" s="42" t="s">
-        <v>167</v>
+        <v>247</v>
       </c>
       <c r="J14" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K14" s="38"/>
       <c r="L14" s="38"/>
       <c r="M14" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N14" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O14" s="38" t="s">
-        <v>170</v>
+        <v>280</v>
       </c>
       <c r="P14" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q14" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R14" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S14" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T14" s="38"/>
       <c r="U14" s="39"/>
       <c r="V14" s="40"/>
       <c r="W14" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3822,54 +3789,54 @@
         <v>44</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E15" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="F15" s="36"/>
+        <v>170</v>
+      </c>
+      <c r="F15" s="37"/>
       <c r="G15" s="37"/>
       <c r="H15" s="37"/>
       <c r="I15" s="42"/>
       <c r="J15" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K15" s="38"/>
       <c r="L15" s="38"/>
       <c r="M15" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N15" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O15" s="38" t="s">
-        <v>173</v>
+        <v>281</v>
       </c>
       <c r="P15" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q15" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R15" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S15" s="38" t="s">
-        <v>169</v>
+        <v>284</v>
       </c>
       <c r="T15" s="38"/>
       <c r="U15" s="39" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="V15" s="40"/>
       <c r="W15" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3877,54 +3844,54 @@
         <v>48</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E16" s="43" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
       <c r="H16" s="37"/>
       <c r="I16" s="42"/>
       <c r="J16" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K16" s="38"/>
       <c r="L16" s="38"/>
       <c r="M16" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N16" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O16" s="38" t="s">
-        <v>173</v>
+        <v>281</v>
       </c>
       <c r="P16" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q16" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R16" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S16" s="38" t="s">
-        <v>169</v>
+        <v>284</v>
       </c>
       <c r="T16" s="38"/>
       <c r="U16" s="39" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="V16" s="40"/>
       <c r="W16" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3932,60 +3899,60 @@
         <v>53</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="E17" s="43" t="s">
-        <v>152</v>
-      </c>
-      <c r="F17" s="36">
+        <v>159</v>
+      </c>
+      <c r="F17" s="37">
         <v>45945</v>
       </c>
       <c r="G17" s="37" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H17" s="37" t="s">
-        <v>183</v>
+        <v>215</v>
       </c>
       <c r="I17" s="42" t="s">
-        <v>184</v>
+        <v>248</v>
       </c>
       <c r="J17" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K17" s="38"/>
       <c r="L17" s="38"/>
       <c r="M17" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N17" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O17" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P17" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q17" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R17" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S17" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T17" s="38"/>
       <c r="U17" s="39"/>
       <c r="V17" s="40"/>
       <c r="W17" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3993,60 +3960,60 @@
         <v>55</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C18" s="41" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E18" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="36">
+        <v>58</v>
+      </c>
+      <c r="F18" s="37">
         <v>45945</v>
       </c>
       <c r="G18" s="37" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H18" s="37" t="s">
-        <v>186</v>
+        <v>216</v>
       </c>
       <c r="I18" s="42" t="s">
-        <v>187</v>
+        <v>249</v>
       </c>
       <c r="J18" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K18" s="38"/>
       <c r="L18" s="38"/>
       <c r="M18" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N18" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O18" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P18" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q18" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R18" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S18" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T18" s="38"/>
       <c r="U18" s="39"/>
       <c r="V18" s="40"/>
       <c r="W18" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4054,60 +4021,60 @@
         <v>56</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E19" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" s="36">
+        <v>60</v>
+      </c>
+      <c r="F19" s="37">
         <v>45945</v>
       </c>
       <c r="G19" s="37" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="H19" s="37" t="s">
-        <v>189</v>
+        <v>217</v>
       </c>
       <c r="I19" s="42" t="s">
-        <v>190</v>
+        <v>250</v>
       </c>
       <c r="J19" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K19" s="38"/>
       <c r="L19" s="38"/>
       <c r="M19" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N19" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O19" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P19" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q19" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R19" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S19" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T19" s="38"/>
       <c r="U19" s="39"/>
       <c r="V19" s="40"/>
       <c r="W19" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4115,60 +4082,60 @@
         <v>57</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E20" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="F20" s="36">
+        <v>62</v>
+      </c>
+      <c r="F20" s="37">
         <v>45945</v>
       </c>
       <c r="G20" s="37" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="H20" s="37" t="s">
-        <v>192</v>
+        <v>218</v>
       </c>
       <c r="I20" s="42" t="s">
-        <v>193</v>
+        <v>251</v>
       </c>
       <c r="J20" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K20" s="38"/>
       <c r="L20" s="38"/>
       <c r="M20" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N20" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O20" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P20" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q20" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R20" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S20" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T20" s="38"/>
       <c r="U20" s="39"/>
       <c r="V20" s="40"/>
       <c r="W20" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4176,60 +4143,60 @@
         <v>59</v>
       </c>
       <c r="B21" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C21" s="41" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E21" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="36">
+        <v>64</v>
+      </c>
+      <c r="F21" s="37">
         <v>45945</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H21" s="37" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="I21" s="42" t="s">
-        <v>196</v>
+        <v>252</v>
       </c>
       <c r="J21" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K21" s="38"/>
       <c r="L21" s="38"/>
       <c r="M21" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N21" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O21" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P21" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q21" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R21" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S21" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T21" s="38"/>
       <c r="U21" s="39"/>
       <c r="V21" s="40"/>
       <c r="W21" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4237,60 +4204,60 @@
         <v>60</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C22" s="41" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E22" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" s="36">
+        <v>66</v>
+      </c>
+      <c r="F22" s="37">
         <v>45945</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="H22" s="37" t="s">
-        <v>199</v>
+        <v>220</v>
       </c>
       <c r="I22" s="42" t="s">
-        <v>198</v>
+        <v>253</v>
       </c>
       <c r="J22" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K22" s="38"/>
       <c r="L22" s="38"/>
       <c r="M22" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N22" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O22" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P22" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q22" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R22" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S22" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T22" s="38"/>
       <c r="U22" s="39"/>
       <c r="V22" s="40"/>
       <c r="W22" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4298,60 +4265,60 @@
         <v>61</v>
       </c>
       <c r="B23" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C23" s="41" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E23" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" s="36">
+        <v>68</v>
+      </c>
+      <c r="F23" s="37">
         <v>45945</v>
       </c>
       <c r="G23" s="37" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="H23" s="37" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
       <c r="I23" s="42" t="s">
-        <v>202</v>
+        <v>254</v>
       </c>
       <c r="J23" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K23" s="38"/>
       <c r="L23" s="38"/>
       <c r="M23" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N23" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O23" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P23" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q23" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R23" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S23" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T23" s="38"/>
       <c r="U23" s="39"/>
       <c r="V23" s="40"/>
       <c r="W23" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4359,60 +4326,60 @@
         <v>62</v>
       </c>
       <c r="B24" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C24" s="41" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E24" s="43" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" s="36">
+        <v>70</v>
+      </c>
+      <c r="F24" s="37">
         <v>45945</v>
       </c>
       <c r="G24" s="37" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="H24" s="37" t="s">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="I24" s="42" t="s">
-        <v>205</v>
+        <v>255</v>
       </c>
       <c r="J24" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K24" s="38"/>
       <c r="L24" s="38"/>
       <c r="M24" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N24" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O24" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P24" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q24" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R24" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S24" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T24" s="38"/>
       <c r="U24" s="39"/>
       <c r="V24" s="40"/>
       <c r="W24" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4420,60 +4387,60 @@
         <v>152</v>
       </c>
       <c r="B25" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C25" s="41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D25" s="35" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E25" s="43" t="s">
-        <v>120</v>
-      </c>
-      <c r="F25" s="36">
+        <v>125</v>
+      </c>
+      <c r="F25" s="37">
         <v>45945</v>
       </c>
       <c r="G25" s="37" t="s">
-        <v>213</v>
+        <v>187</v>
       </c>
       <c r="H25" s="37" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="I25" s="42" t="s">
-        <v>215</v>
+        <v>256</v>
       </c>
       <c r="J25" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K25" s="38"/>
       <c r="L25" s="38"/>
       <c r="M25" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N25" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O25" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P25" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q25" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R25" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S25" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T25" s="38"/>
       <c r="U25" s="39"/>
       <c r="V25" s="40"/>
       <c r="W25" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4481,60 +4448,60 @@
         <v>154</v>
       </c>
       <c r="B26" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C26" s="41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D26" s="35" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E26" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="F26" s="36">
+        <v>126</v>
+      </c>
+      <c r="F26" s="37">
         <v>45945</v>
       </c>
       <c r="G26" s="37" t="s">
-        <v>216</v>
+        <v>188</v>
       </c>
       <c r="H26" s="37" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="I26" s="42" t="s">
-        <v>218</v>
+        <v>257</v>
       </c>
       <c r="J26" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K26" s="38"/>
       <c r="L26" s="38"/>
       <c r="M26" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N26" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O26" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P26" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q26" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R26" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S26" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T26" s="38"/>
       <c r="U26" s="39"/>
       <c r="V26" s="40"/>
       <c r="W26" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4542,60 +4509,60 @@
         <v>155</v>
       </c>
       <c r="B27" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C27" s="41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D27" s="35" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E27" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="F27" s="36">
+        <v>127</v>
+      </c>
+      <c r="F27" s="37">
         <v>45945</v>
       </c>
       <c r="G27" s="37" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="H27" s="37" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="I27" s="42" t="s">
-        <v>221</v>
+        <v>258</v>
       </c>
       <c r="J27" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K27" s="38"/>
       <c r="L27" s="38"/>
       <c r="M27" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N27" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O27" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P27" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q27" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R27" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S27" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T27" s="38"/>
       <c r="U27" s="39"/>
       <c r="V27" s="40"/>
       <c r="W27" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4603,60 +4570,60 @@
         <v>156</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C28" s="41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E28" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="F28" s="36">
+        <v>128</v>
+      </c>
+      <c r="F28" s="37">
         <v>45945</v>
       </c>
       <c r="G28" s="37" t="s">
-        <v>222</v>
+        <v>190</v>
       </c>
       <c r="H28" s="37" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="I28" s="42" t="s">
-        <v>224</v>
+        <v>259</v>
       </c>
       <c r="J28" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K28" s="38"/>
       <c r="L28" s="38"/>
       <c r="M28" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N28" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O28" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P28" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q28" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R28" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S28" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T28" s="38"/>
       <c r="U28" s="39"/>
       <c r="V28" s="40"/>
       <c r="W28" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4664,60 +4631,60 @@
         <v>159</v>
       </c>
       <c r="B29" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C29" s="41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D29" s="35" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E29" s="43" t="s">
-        <v>73</v>
-      </c>
-      <c r="F29" s="36">
+        <v>76</v>
+      </c>
+      <c r="F29" s="37">
         <v>45945</v>
       </c>
       <c r="G29" s="37" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="H29" s="37" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="I29" s="42" t="s">
-        <v>227</v>
+        <v>260</v>
       </c>
       <c r="J29" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K29" s="38"/>
       <c r="L29" s="38"/>
       <c r="M29" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N29" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O29" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P29" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q29" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R29" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S29" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T29" s="38"/>
       <c r="U29" s="39"/>
       <c r="V29" s="40"/>
       <c r="W29" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4725,60 +4692,60 @@
         <v>160</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C30" s="41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E30" s="43" t="s">
-        <v>75</v>
-      </c>
-      <c r="F30" s="36">
+        <v>78</v>
+      </c>
+      <c r="F30" s="37">
         <v>45945</v>
       </c>
       <c r="G30" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="H30" s="37" t="s">
         <v>228</v>
       </c>
-      <c r="H30" s="37" t="s">
-        <v>229</v>
-      </c>
       <c r="I30" s="42" t="s">
-        <v>230</v>
+        <v>261</v>
       </c>
       <c r="J30" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K30" s="38"/>
       <c r="L30" s="38"/>
       <c r="M30" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N30" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O30" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P30" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q30" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R30" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S30" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T30" s="38"/>
       <c r="U30" s="39"/>
       <c r="V30" s="40"/>
       <c r="W30" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4786,60 +4753,60 @@
         <v>161</v>
       </c>
       <c r="B31" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C31" s="41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D31" s="35" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E31" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="F31" s="36">
+        <v>116</v>
+      </c>
+      <c r="F31" s="37">
         <v>45945</v>
       </c>
       <c r="G31" s="37" t="s">
-        <v>231</v>
+        <v>193</v>
       </c>
       <c r="H31" s="37" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I31" s="42" t="s">
-        <v>233</v>
+        <v>262</v>
       </c>
       <c r="J31" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K31" s="38"/>
       <c r="L31" s="38"/>
       <c r="M31" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N31" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O31" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P31" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q31" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R31" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S31" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T31" s="38"/>
       <c r="U31" s="39"/>
       <c r="V31" s="40"/>
       <c r="W31" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4847,60 +4814,60 @@
         <v>162</v>
       </c>
       <c r="B32" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C32" s="41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D32" s="35" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E32" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="F32" s="36">
+        <v>117</v>
+      </c>
+      <c r="F32" s="37">
         <v>45945</v>
       </c>
       <c r="G32" s="37" t="s">
-        <v>234</v>
+        <v>194</v>
       </c>
       <c r="H32" s="37" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="I32" s="42" t="s">
-        <v>236</v>
+        <v>263</v>
       </c>
       <c r="J32" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K32" s="38"/>
       <c r="L32" s="38"/>
       <c r="M32" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N32" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O32" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P32" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q32" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R32" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S32" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T32" s="38"/>
       <c r="U32" s="39"/>
       <c r="V32" s="40"/>
       <c r="W32" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4908,60 +4875,60 @@
         <v>163</v>
       </c>
       <c r="B33" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C33" s="41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D33" s="35" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E33" s="43" t="s">
-        <v>113</v>
-      </c>
-      <c r="F33" s="36">
+        <v>118</v>
+      </c>
+      <c r="F33" s="37">
         <v>45945</v>
       </c>
       <c r="G33" s="37" t="s">
-        <v>237</v>
+        <v>195</v>
       </c>
       <c r="H33" s="37" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="I33" s="42" t="s">
-        <v>239</v>
+        <v>264</v>
       </c>
       <c r="J33" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K33" s="38"/>
       <c r="L33" s="38"/>
       <c r="M33" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N33" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O33" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P33" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q33" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R33" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S33" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T33" s="38"/>
       <c r="U33" s="39"/>
       <c r="V33" s="40"/>
       <c r="W33" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4969,60 +4936,60 @@
         <v>164</v>
       </c>
       <c r="B34" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C34" s="41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D34" s="35" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E34" s="43" t="s">
-        <v>114</v>
-      </c>
-      <c r="F34" s="36">
+        <v>119</v>
+      </c>
+      <c r="F34" s="37">
         <v>45945</v>
       </c>
       <c r="G34" s="37" t="s">
-        <v>242</v>
+        <v>196</v>
       </c>
       <c r="H34" s="37" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="I34" s="42" t="s">
-        <v>241</v>
+        <v>265</v>
       </c>
       <c r="J34" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K34" s="38"/>
       <c r="L34" s="38"/>
       <c r="M34" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N34" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O34" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P34" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q34" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R34" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S34" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T34" s="38"/>
       <c r="U34" s="39"/>
       <c r="V34" s="40"/>
       <c r="W34" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5030,60 +4997,60 @@
         <v>165</v>
       </c>
       <c r="B35" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C35" s="41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D35" s="35" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E35" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="F35" s="36">
+        <v>120</v>
+      </c>
+      <c r="F35" s="37">
         <v>45945</v>
       </c>
       <c r="G35" s="37" t="s">
-        <v>243</v>
+        <v>197</v>
       </c>
       <c r="H35" s="37" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="I35" s="42" t="s">
-        <v>244</v>
+        <v>266</v>
       </c>
       <c r="J35" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K35" s="38"/>
       <c r="L35" s="38"/>
       <c r="M35" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N35" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O35" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P35" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q35" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R35" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S35" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T35" s="38"/>
       <c r="U35" s="39"/>
       <c r="V35" s="40"/>
       <c r="W35" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5091,60 +5058,60 @@
         <v>166</v>
       </c>
       <c r="B36" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C36" s="41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D36" s="35" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E36" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="F36" s="36">
+        <v>121</v>
+      </c>
+      <c r="F36" s="37">
         <v>45945</v>
       </c>
       <c r="G36" s="37" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
       <c r="H36" s="37" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="I36" s="42" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
       <c r="J36" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K36" s="38"/>
       <c r="L36" s="38"/>
       <c r="M36" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N36" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O36" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P36" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q36" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R36" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S36" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T36" s="38"/>
       <c r="U36" s="39"/>
       <c r="V36" s="40"/>
       <c r="W36" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5152,60 +5119,60 @@
         <v>167</v>
       </c>
       <c r="B37" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C37" s="41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D37" s="35" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E37" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="F37" s="36">
+        <v>122</v>
+      </c>
+      <c r="F37" s="37">
         <v>45945</v>
       </c>
       <c r="G37" s="37" t="s">
-        <v>249</v>
+        <v>199</v>
       </c>
       <c r="H37" s="37" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="I37" s="42" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
       <c r="J37" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K37" s="38"/>
       <c r="L37" s="38"/>
       <c r="M37" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N37" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O37" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P37" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q37" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R37" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S37" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T37" s="38"/>
       <c r="U37" s="39"/>
       <c r="V37" s="40"/>
       <c r="W37" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5213,60 +5180,60 @@
         <v>168</v>
       </c>
       <c r="B38" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C38" s="41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D38" s="35" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E38" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="F38" s="36">
+        <v>123</v>
+      </c>
+      <c r="F38" s="37">
         <v>45945</v>
       </c>
       <c r="G38" s="37" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H38" s="37" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="I38" s="42" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
       <c r="J38" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K38" s="38"/>
       <c r="L38" s="38"/>
       <c r="M38" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N38" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O38" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P38" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q38" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R38" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S38" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T38" s="38"/>
       <c r="U38" s="39"/>
       <c r="V38" s="40"/>
       <c r="W38" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5274,94 +5241,88 @@
         <v>169</v>
       </c>
       <c r="B39" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C39" s="41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D39" s="35" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E39" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="F39" s="36">
+        <v>124</v>
+      </c>
+      <c r="F39" s="37">
         <v>45945</v>
       </c>
       <c r="G39" s="37" t="s">
-        <v>255</v>
+        <v>201</v>
       </c>
       <c r="H39" s="37" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="I39" s="42" t="s">
-        <v>257</v>
+        <v>270</v>
       </c>
       <c r="J39" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K39" s="38"/>
       <c r="L39" s="38"/>
       <c r="M39" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N39" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="O39" s="38" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="P39" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q39" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R39" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S39" s="38" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="T39" s="38"/>
       <c r="U39" s="39"/>
       <c r="V39" s="40"/>
       <c r="W39" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="35">
-        <v>448</v>
+        <v>191</v>
       </c>
       <c r="B40" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C40" s="41" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D40" s="35" t="s">
-        <v>133</v>
+        <v>88</v>
       </c>
       <c r="E40" s="43" t="s">
-        <v>135</v>
-      </c>
-      <c r="F40" s="36">
-        <v>45946</v>
-      </c>
-      <c r="G40" s="37" t="s">
-        <v>269</v>
-      </c>
-      <c r="H40" s="37" t="s">
-        <v>267</v>
-      </c>
-      <c r="I40" s="42" t="s">
-        <v>268</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="42"/>
       <c r="J40" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="K40" s="38"/>
+        <v>98</v>
+      </c>
+      <c r="K40" s="45" t="s">
+        <v>285</v>
+      </c>
       <c r="L40" s="38"/>
       <c r="M40" s="38"/>
       <c r="N40" s="38"/>
@@ -5374,41 +5335,35 @@
       <c r="U40" s="39"/>
       <c r="V40" s="40"/>
       <c r="W40" s="38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="41" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="35">
-        <v>449</v>
+        <v>376</v>
       </c>
       <c r="B41" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C41" s="41" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D41" s="35" t="s">
-        <v>134</v>
+        <v>89</v>
       </c>
       <c r="E41" s="43" t="s">
-        <v>136</v>
-      </c>
-      <c r="F41" s="36">
-        <v>45946</v>
-      </c>
-      <c r="G41" s="37" t="s">
-        <v>272</v>
-      </c>
-      <c r="H41" s="37" t="s">
-        <v>270</v>
-      </c>
-      <c r="I41" s="42" t="s">
-        <v>271</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="42"/>
       <c r="J41" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="K41" s="38"/>
+        <v>98</v>
+      </c>
+      <c r="K41" s="45" t="s">
+        <v>285</v>
+      </c>
       <c r="L41" s="38"/>
       <c r="M41" s="38"/>
       <c r="N41" s="38"/>
@@ -5421,39 +5376,39 @@
       <c r="U41" s="39"/>
       <c r="V41" s="40"/>
       <c r="W41" s="38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="35">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B42" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C42" s="41" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="D42" s="35" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="E42" s="43" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="F42" s="37">
         <v>45946</v>
       </c>
       <c r="G42" s="37" t="s">
-        <v>278</v>
+        <v>202</v>
       </c>
       <c r="H42" s="37" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="I42" s="42" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="J42" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K42" s="38"/>
       <c r="L42" s="38"/>
@@ -5468,355 +5423,409 @@
       <c r="U42" s="39"/>
       <c r="V42" s="40"/>
       <c r="W42" s="38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="35">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="B43" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C43" s="41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D43" s="35" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E43" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="F43" s="37">
+        <v>45946</v>
+      </c>
+      <c r="G43" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="H43" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="I43" s="42" t="s">
+        <v>272</v>
+      </c>
+      <c r="J43" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="K43" s="38"/>
+      <c r="L43" s="38"/>
+      <c r="M43" s="38"/>
+      <c r="N43" s="38"/>
+      <c r="O43" s="38"/>
+      <c r="P43" s="38"/>
+      <c r="Q43" s="38"/>
+      <c r="R43" s="38"/>
+      <c r="S43" s="38"/>
+      <c r="T43" s="38"/>
+      <c r="U43" s="39"/>
+      <c r="V43" s="40"/>
+      <c r="W43" s="38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="35">
+        <v>452</v>
+      </c>
+      <c r="B44" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D44" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="E44" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="F43" s="36">
-        <v>45945</v>
-      </c>
-      <c r="G43" s="35" t="s">
-        <v>258</v>
-      </c>
-      <c r="H43" s="35" t="s">
-        <v>259</v>
-      </c>
-      <c r="I43" s="35" t="s">
-        <v>260</v>
-      </c>
-      <c r="J43" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="K43" s="38"/>
-      <c r="L43" s="35"/>
-      <c r="M43" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="N43" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="O43" s="38" t="s">
-        <v>171</v>
-      </c>
-      <c r="P43" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q43" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="R43" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="S43" s="38" t="s">
-        <v>168</v>
-      </c>
-      <c r="T43" s="38"/>
-      <c r="U43" s="35"/>
-      <c r="V43" s="35"/>
-      <c r="W43" s="35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="35">
-        <v>466</v>
-      </c>
-      <c r="B44" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C44" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="D44" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="E44" s="44" t="s">
-        <v>150</v>
-      </c>
-      <c r="F44" s="36">
-        <v>45945</v>
-      </c>
-      <c r="G44" s="35" t="s">
-        <v>207</v>
-      </c>
-      <c r="H44" s="35" t="s">
-        <v>208</v>
-      </c>
-      <c r="I44" s="35" t="s">
-        <v>209</v>
+      <c r="F44" s="37">
+        <v>45946</v>
+      </c>
+      <c r="G44" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="H44" s="37" t="s">
+        <v>240</v>
+      </c>
+      <c r="I44" s="42" t="s">
+        <v>273</v>
       </c>
       <c r="J44" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K44" s="38"/>
-      <c r="L44" s="35"/>
-      <c r="M44" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="N44" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="O44" s="38" t="s">
-        <v>171</v>
-      </c>
-      <c r="P44" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q44" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="R44" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="S44" s="38" t="s">
-        <v>168</v>
-      </c>
+      <c r="L44" s="38"/>
+      <c r="M44" s="38"/>
+      <c r="N44" s="38"/>
+      <c r="O44" s="38"/>
+      <c r="P44" s="38"/>
+      <c r="Q44" s="38"/>
+      <c r="R44" s="38"/>
+      <c r="S44" s="38"/>
       <c r="T44" s="38"/>
-      <c r="U44" s="35"/>
-      <c r="V44" s="35"/>
-      <c r="W44" s="35" t="s">
-        <v>44</v>
+      <c r="U44" s="39"/>
+      <c r="V44" s="40"/>
+      <c r="W44" s="38" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B45" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C45" s="41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D45" s="35" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="E45" s="43" t="s">
-        <v>142</v>
-      </c>
-      <c r="F45" s="36">
+        <v>144</v>
+      </c>
+      <c r="F45" s="35">
         <v>45945</v>
       </c>
       <c r="G45" s="35" t="s">
-        <v>261</v>
+        <v>205</v>
       </c>
       <c r="H45" s="35" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
       <c r="I45" s="35" t="s">
-        <v>263</v>
+        <v>274</v>
       </c>
       <c r="J45" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K45" s="38"/>
       <c r="L45" s="35"/>
       <c r="M45" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N45" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="O45" s="38" t="s">
-        <v>171</v>
+        <v>55</v>
+      </c>
+      <c r="O45" s="35" t="s">
+        <v>282</v>
       </c>
       <c r="P45" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q45" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R45" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="S45" s="38" t="s">
-        <v>168</v>
+        <v>55</v>
+      </c>
+      <c r="S45" s="35" t="s">
+        <v>283</v>
       </c>
       <c r="T45" s="38"/>
       <c r="U45" s="35"/>
       <c r="V45" s="35"/>
       <c r="W45" s="35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="35">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="B46" s="35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C46" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="D46" s="41" t="s">
-        <v>156</v>
-      </c>
-      <c r="E46" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="D46" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="E46" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="F46" s="37">
+      <c r="F46" s="35">
         <v>45945</v>
       </c>
-      <c r="G46" s="37" t="s">
-        <v>210</v>
-      </c>
-      <c r="H46" s="37" t="s">
-        <v>212</v>
-      </c>
-      <c r="I46" s="42" t="s">
-        <v>211</v>
+      <c r="G46" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="H46" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="I46" s="35" t="s">
+        <v>275</v>
       </c>
       <c r="J46" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K46" s="38"/>
-      <c r="L46" s="38"/>
+      <c r="L46" s="35"/>
       <c r="M46" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N46" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="O46" s="38" t="s">
-        <v>171</v>
+        <v>55</v>
+      </c>
+      <c r="O46" s="35" t="s">
+        <v>282</v>
       </c>
       <c r="P46" s="38" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q46" s="38" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R46" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="S46" s="38" t="s">
-        <v>168</v>
+        <v>55</v>
+      </c>
+      <c r="S46" s="35" t="s">
+        <v>283</v>
       </c>
       <c r="T46" s="38"/>
-      <c r="U46" s="39"/>
-      <c r="V46" s="40"/>
-      <c r="W46" s="38" t="s">
-        <v>44</v>
+      <c r="U46" s="35"/>
+      <c r="V46" s="35"/>
+      <c r="W46" s="35" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="35">
+        <v>468</v>
+      </c>
+      <c r="B47" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="E47" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="F47" s="35">
+        <v>45945</v>
+      </c>
+      <c r="G47" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="H47" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="I47" s="35" t="s">
+        <v>276</v>
+      </c>
+      <c r="J47" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="K47" s="38"/>
+      <c r="L47" s="35"/>
+      <c r="M47" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="N47" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="O47" s="35" t="s">
+        <v>282</v>
+      </c>
+      <c r="P47" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q47" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="R47" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="S47" s="35" t="s">
+        <v>283</v>
+      </c>
+      <c r="T47" s="38"/>
+      <c r="U47" s="35"/>
+      <c r="V47" s="35"/>
+      <c r="W47" s="35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="35">
+        <v>473</v>
+      </c>
+      <c r="B48" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D48" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="E48" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="F48" s="37">
+        <v>45945</v>
+      </c>
+      <c r="G48" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="H48" s="37" t="s">
+        <v>244</v>
+      </c>
+      <c r="I48" s="42" t="s">
+        <v>277</v>
+      </c>
+      <c r="J48" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="K48" s="38"/>
+      <c r="L48" s="38"/>
+      <c r="M48" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="N48" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="O48" s="38" t="s">
+        <v>282</v>
+      </c>
+      <c r="P48" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q48" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="R48" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="S48" s="38" t="s">
+        <v>283</v>
+      </c>
+      <c r="T48" s="38"/>
+      <c r="U48" s="39"/>
+      <c r="V48" s="40"/>
+      <c r="W48" s="38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="35">
         <v>475</v>
       </c>
-      <c r="B47" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C47" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="D47" s="35" t="s">
-        <v>155</v>
-      </c>
-      <c r="E47" s="43" t="s">
-        <v>158</v>
-      </c>
-      <c r="F47" s="37">
+      <c r="B49" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="E49" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="F49" s="37">
         <v>45945</v>
       </c>
-      <c r="G47" s="37" t="s">
-        <v>264</v>
-      </c>
-      <c r="H47" s="37" t="s">
-        <v>265</v>
-      </c>
-      <c r="I47" s="42" t="s">
-        <v>266</v>
-      </c>
-      <c r="J47" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="K47" s="38"/>
-      <c r="L47" s="38"/>
-      <c r="M47" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="N47" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="O47" s="38" t="s">
-        <v>171</v>
-      </c>
-      <c r="P47" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q47" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="R47" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="S47" s="38" t="s">
-        <v>168</v>
-      </c>
-      <c r="T47" s="38"/>
-      <c r="U47" s="39"/>
-      <c r="V47" s="40"/>
-      <c r="W47" s="38" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="48" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
-      <c r="L48" s="7"/>
-      <c r="M48" s="7"/>
-      <c r="N48" s="7"/>
-      <c r="O48" s="7"/>
-      <c r="P48" s="7"/>
-      <c r="Q48" s="7"/>
-      <c r="R48" s="7"/>
-      <c r="S48" s="7"/>
-      <c r="T48" s="7"/>
-      <c r="U48" s="8"/>
-      <c r="V48" s="2"/>
-      <c r="W48" s="9"/>
-    </row>
-    <row r="49" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="7"/>
-      <c r="M49" s="7"/>
-      <c r="N49" s="7"/>
-      <c r="O49" s="7"/>
-      <c r="P49" s="7"/>
-      <c r="Q49" s="7"/>
-      <c r="R49" s="7"/>
-      <c r="S49" s="7"/>
-      <c r="T49" s="7"/>
-      <c r="U49" s="8"/>
-      <c r="V49" s="2"/>
-      <c r="W49" s="9"/>
-    </row>
-    <row r="50" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G49" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="H49" s="37" t="s">
+        <v>245</v>
+      </c>
+      <c r="I49" s="42" t="s">
+        <v>278</v>
+      </c>
+      <c r="J49" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="K49" s="38"/>
+      <c r="L49" s="38"/>
+      <c r="M49" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="N49" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="O49" s="38" t="s">
+        <v>282</v>
+      </c>
+      <c r="P49" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q49" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="R49" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="S49" s="38" t="s">
+        <v>283</v>
+      </c>
+      <c r="T49" s="38"/>
+      <c r="U49" s="39"/>
+      <c r="V49" s="40"/>
+      <c r="W49" s="38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
@@ -5836,7 +5845,7 @@
       <c r="V50" s="2"/>
       <c r="W50" s="9"/>
     </row>
-    <row r="51" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
@@ -5856,7 +5865,7 @@
       <c r="V51" s="2"/>
       <c r="W51" s="9"/>
     </row>
-    <row r="52" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
@@ -5876,7 +5885,7 @@
       <c r="V52" s="2"/>
       <c r="W52" s="9"/>
     </row>
-    <row r="53" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
@@ -5896,7 +5905,7 @@
       <c r="V53" s="2"/>
       <c r="W53" s="9"/>
     </row>
-    <row r="54" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
       <c r="H54" s="6"/>
@@ -5916,7 +5925,7 @@
       <c r="V54" s="2"/>
       <c r="W54" s="9"/>
     </row>
-    <row r="55" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
@@ -5936,7 +5945,7 @@
       <c r="V55" s="2"/>
       <c r="W55" s="9"/>
     </row>
-    <row r="56" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
@@ -5956,7 +5965,7 @@
       <c r="V56" s="2"/>
       <c r="W56" s="9"/>
     </row>
-    <row r="57" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
@@ -5976,7 +5985,7 @@
       <c r="V57" s="2"/>
       <c r="W57" s="9"/>
     </row>
-    <row r="58" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
       <c r="H58" s="6"/>
@@ -5996,7 +6005,7 @@
       <c r="V58" s="2"/>
       <c r="W58" s="9"/>
     </row>
-    <row r="59" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
@@ -6016,7 +6025,7 @@
       <c r="V59" s="2"/>
       <c r="W59" s="9"/>
     </row>
-    <row r="60" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
       <c r="H60" s="6"/>
@@ -6036,7 +6045,7 @@
       <c r="V60" s="2"/>
       <c r="W60" s="9"/>
     </row>
-    <row r="61" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
       <c r="H61" s="6"/>
@@ -6056,7 +6065,7 @@
       <c r="V61" s="2"/>
       <c r="W61" s="9"/>
     </row>
-    <row r="62" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
       <c r="H62" s="6"/>
@@ -6076,7 +6085,7 @@
       <c r="V62" s="2"/>
       <c r="W62" s="9"/>
     </row>
-    <row r="63" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
       <c r="H63" s="6"/>
@@ -6096,7 +6105,7 @@
       <c r="V63" s="2"/>
       <c r="W63" s="9"/>
     </row>
-    <row r="64" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
       <c r="H64" s="6"/>
@@ -8537,10 +8546,44 @@
       <c r="W185" s="9"/>
     </row>
     <row r="186" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="W186" s="7"/>
+      <c r="F186" s="6"/>
+      <c r="G186" s="6"/>
+      <c r="H186" s="6"/>
+      <c r="I186" s="6"/>
+      <c r="J186" s="7"/>
+      <c r="K186" s="7"/>
+      <c r="L186" s="7"/>
+      <c r="M186" s="7"/>
+      <c r="N186" s="7"/>
+      <c r="O186" s="7"/>
+      <c r="P186" s="7"/>
+      <c r="Q186" s="7"/>
+      <c r="R186" s="7"/>
+      <c r="S186" s="7"/>
+      <c r="T186" s="7"/>
+      <c r="U186" s="8"/>
+      <c r="V186" s="2"/>
+      <c r="W186" s="9"/>
     </row>
     <row r="187" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="W187" s="7"/>
+      <c r="F187" s="6"/>
+      <c r="G187" s="6"/>
+      <c r="H187" s="6"/>
+      <c r="I187" s="6"/>
+      <c r="J187" s="7"/>
+      <c r="K187" s="7"/>
+      <c r="L187" s="7"/>
+      <c r="M187" s="7"/>
+      <c r="N187" s="7"/>
+      <c r="O187" s="7"/>
+      <c r="P187" s="7"/>
+      <c r="Q187" s="7"/>
+      <c r="R187" s="7"/>
+      <c r="S187" s="7"/>
+      <c r="T187" s="7"/>
+      <c r="U187" s="8"/>
+      <c r="V187" s="2"/>
+      <c r="W187" s="9"/>
     </row>
     <row r="188" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="W188" s="7"/>
@@ -9787,13 +9830,19 @@
     <row r="602" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="W602" s="7"/>
     </row>
-    <row r="603" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W603" s="7"/>
+    </row>
+    <row r="604" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W604" s="7"/>
+    </row>
     <row r="605" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="606" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="607" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A9:W47"/>
+  <autoFilter ref="A9:W49"/>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
@@ -9814,19 +9863,19 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P10:R47 M10:N47 J10:J47</xm:sqref>
+          <xm:sqref>M10:N49 J10:J49 P10:R49</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>T10:T47</xm:sqref>
+          <xm:sqref>T10:T49</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'LISTA VALORI'!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>K10:K47</xm:sqref>
+          <xm:sqref>K10:K39 K42:K49</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -9846,42 +9895,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -9911,162 +9960,162 @@
   <sheetData>
     <row r="1" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11044,26 +11093,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12089,6 +12138,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -12346,15 +12404,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
@@ -12373,6 +12422,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12391,14 +12448,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Aggiunta motivazione non applicabilità
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#MDATECHNOLOGYSRLXX/MDA_TECHNOLOGY/SOILAB_Innovative/13.8.5/report-checklist.xlsx
+++ b/GATEWAY/A1#111#MDATECHNOLOGYSRLXX/MDA_TECHNOLOGY/SOILAB_Innovative/13.8.5/report-checklist.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="285">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1127,9 +1127,6 @@
   </si>
   <si>
     <t>Si eseguono altri tentativi di trasmissione del documento</t>
-  </si>
-  <si>
-    <t>I laboratori di analisi che utilizzano il nostro software sono laboratori di base con settori specializzati di tipo ambulatoriale e non ospedaliero. Nei punti prelievo di questi laboratori accedono cittadini che devono fare controlli di prevenzione e in nessuno di essi sono svolte attività di trasfusione, per le quali servono specifici atti autorizzativi che non rientrano tra quelli in possesso dalla nostra clientela.</t>
   </si>
 </sst>
 </file>
@@ -1612,7 +1609,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1732,7 +1729,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1754,6 +1750,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3205,10 +3207,10 @@
   <dimension ref="A1:W609"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3250,12 +3252,12 @@
       <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="49"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="48"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -3276,14 +3278,14 @@
       <c r="W2" s="9"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="57" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="48"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -3304,12 +3306,12 @@
       <c r="W3" s="9"/>
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="57" t="s">
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="49"/>
+      <c r="D4" s="48"/>
       <c r="E4" s="4"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -3331,12 +3333,12 @@
       <c r="W4" s="9"/>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="55"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="57" t="s">
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="48"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -3357,8 +3359,8 @@
       <c r="W5" s="9"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="47"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="10"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -5320,10 +5322,10 @@
       <c r="J40" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="K40" s="45" t="s">
-        <v>285</v>
-      </c>
-      <c r="L40" s="38"/>
+      <c r="K40" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="L40" s="58"/>
       <c r="M40" s="38"/>
       <c r="N40" s="38"/>
       <c r="O40" s="38"/>
@@ -5361,10 +5363,10 @@
       <c r="J41" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="K41" s="45" t="s">
-        <v>285</v>
-      </c>
-      <c r="L41" s="38"/>
+      <c r="K41" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="L41" s="57"/>
       <c r="M41" s="38"/>
       <c r="N41" s="38"/>
       <c r="O41" s="38"/>
@@ -9875,7 +9877,7 @@
           <x14:formula1>
             <xm:f>'LISTA VALORI'!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>K10:K39 K42:K49</xm:sqref>
+          <xm:sqref>K10:K49</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -12126,6 +12128,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
@@ -12135,15 +12146,6 @@
     <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12405,6 +12407,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -12417,14 +12427,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>